<commit_message>
Zeiterfassung_Musliu_Leon.xlsx: Eintragen meiner Zeiten
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Musliu_Leon.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Musliu_Leon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\FR1PEPF00000B6B\EXCELCNV\463d9eba-11c2-4156-af66-4b4fef8b0f49\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\S5\SOPR\RaytRazor\1. Projektplanung\1.1 Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{6E1620ED-6CE1-4223-B022-CA90046BE70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA5961FC-EDCD-46CF-A215-02FBB907FCE5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A51909D-C2E9-4A6A-AEA4-D472F0852A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{D8EBEC6F-97AA-4447-BC60-E9767B6B54BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D8EBEC6F-97AA-4447-BC60-E9767B6B54BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Name:</t>
   </si>
@@ -47,9 +47,6 @@
     <t>MatrNr:</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Projekt:</t>
   </si>
   <si>
@@ -75,13 +72,58 @@
   </si>
   <si>
     <t>Teilnahme am Kickoff-Meeting</t>
+  </si>
+  <si>
+    <t>Rayforge</t>
+  </si>
+  <si>
+    <t>Online-Meeting</t>
+  </si>
+  <si>
+    <t>Projekt Kickoff Meeting</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t>Bezüglich .obj / .mtl Dateien</t>
+  </si>
+  <si>
+    <t>Weekly-Summup-01 Meeting</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Erste Ansätze im Java Object Parser</t>
+  </si>
+  <si>
+    <t>Emergency-Meeting</t>
+  </si>
+  <si>
+    <t>Emergency-Meeting abgehalten. (Mail von Management missverstanden)</t>
+  </si>
+  <si>
+    <t>Umschreiben des Object Parsers</t>
+  </si>
+  <si>
+    <t>Bezüglich .obj / .mtl Dateien und erstellen einer Powerpoint für Teammitglieder</t>
+  </si>
+  <si>
+    <t>Fertigstellen des Object Parser Prototyps</t>
+  </si>
+  <si>
+    <t>Präsentation meiner .obj / .mtl Informationen und meines Prototyps</t>
+  </si>
+  <si>
+    <t>Auseinandersetzen mit neuem OpenGL Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -430,22 +472,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A25EDDD-CE0E-4D64-955D-F29BB8D2CC7C}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="256" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="64.7265625" customWidth="1"/>
+    <col min="5" max="256" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -453,45 +495,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="6">
+        <v>3139954</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>45574</v>
       </c>
@@ -499,10 +541,164 @@
         <v>1.5</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>45579</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>45580</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>45583</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>45586</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>45586</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>45587</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>45589</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>45591</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>45592</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>45593</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45593</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -514,6 +710,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EA32FAADEF28B246BE81F09370D9BDD6" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee5e8cab159ec08823d71aeff920ea58">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcfc458b-b0e2-47b4-8909-d39697dfebcc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6553d0449cd115c0021964cc0df6b6b1" ns2:_="">
     <xsd:import namespace="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
@@ -657,29 +868,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9FC6350-6490-4AE5-84BE-162C5C4694A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CEBEC-8504-4D29-B496-720D2223E402}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71F94882-FD0A-418D-8AE4-25897563B4A0}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CEBEC-8504-4D29-B496-720D2223E402}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9FC6350-6490-4AE5-84BE-162C5C4694A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71F94882-FD0A-418D-8AE4-25897563B4A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Zeiterfassung_Musliu_Leon.xlsx: Updates für meine Zeiten
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Musliu_Leon.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Musliu_Leon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\S5\SOPR\RaytRazor\1. Projektplanung\1.1 Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A51909D-C2E9-4A6A-AEA4-D472F0852A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967736E3-289A-4F50-9268-433485EC09E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D8EBEC6F-97AA-4447-BC60-E9767B6B54BF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Name:</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>Auseinandersetzen mit neuem OpenGL Code</t>
+  </si>
+  <si>
+    <t>Objektparser programmieren</t>
+  </si>
+  <si>
+    <t>Objektparser fertigstellen &amp; Materialparser programmieren</t>
+  </si>
+  <si>
+    <t>Materialparser fertigstellen</t>
+  </si>
+  <si>
+    <t>Weekly-Summup-03 Meeting</t>
   </si>
 </sst>
 </file>
@@ -472,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A25EDDD-CE0E-4D64-955D-F29BB8D2CC7C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -701,6 +713,62 @@
         <v>26</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>45597</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>45598</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>45599</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>45600</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -710,21 +778,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EA32FAADEF28B246BE81F09370D9BDD6" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee5e8cab159ec08823d71aeff920ea58">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcfc458b-b0e2-47b4-8909-d39697dfebcc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6553d0449cd115c0021964cc0df6b6b1" ns2:_="">
     <xsd:import namespace="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
@@ -868,24 +921,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9FC6350-6490-4AE5-84BE-162C5C4694A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CEBEC-8504-4D29-B496-720D2223E402}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71F94882-FD0A-418D-8AE4-25897563B4A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -901,4 +952,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7CEBEC-8504-4D29-B496-720D2223E402}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9FC6350-6490-4AE5-84BE-162C5C4694A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>